<commit_message>
Added new test case and selenium grid architecture
</commit_message>
<xml_diff>
--- a/src/main/java/com/opencart/Resources/TestData_PROD.xlsx
+++ b/src/main/java/com/opencart/Resources/TestData_PROD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amritpal.b.singh\Enterprise Test Framework\enterprise-test-automation-framework\src\main\java\com\opencart\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E4587F-45B0-4805-9CDD-4FCB245B019B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24978930-7A33-453F-9B7B-82783FFA174B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Feature</t>
   </si>
@@ -43,10 +43,13 @@
     <t>testenterprise01@mailinator.com</t>
   </si>
   <si>
-    <t>Test@1234</t>
-  </si>
-  <si>
-    <t>Account Details</t>
+    <t>qa_testers@qabrains.com</t>
+  </si>
+  <si>
+    <t>Password123</t>
+  </si>
+  <si>
+    <t>Forgot Password</t>
   </si>
 </sst>
 </file>
@@ -378,17 +381,17 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -399,34 +402,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{F2D2ECB1-3C40-4F5A-9E58-9A2663282FE6}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{F796420F-06E4-4F7C-8867-F25084C11D2E}"/>
-    <hyperlink ref="B2" r:id="rId3" xr:uid="{1930935A-4998-462F-90CD-E8BF4C1B4890}"/>
-    <hyperlink ref="C2" r:id="rId4" xr:uid="{07A8DDAE-CB4F-4D55-9ECD-7C64E92180DE}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{1930935A-4998-462F-90CD-E8BF4C1B4890}"/>
+    <hyperlink ref="C2" r:id="rId3" display="Test@1234" xr:uid="{07A8DDAE-CB4F-4D55-9ECD-7C64E92180DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -438,7 +438,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>